<commit_message>
fixed validated actif format
</commit_message>
<xml_diff>
--- a/outputs/COMPAGNIE_MEDITERRANEENNE_D_ASSURANCES_ET_DE_REASS/COMAR_2024_actif_validated.xlsx
+++ b/outputs/COMPAGNIE_MEDITERRANEENNE_D_ASSURANCES_ET_DE_REASS/COMAR_2024_actif_validated.xlsx
@@ -58,9 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="4" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -512,24 +515,24 @@
         </is>
       </c>
       <c r="E2" s="1" t="n">
-        <v>30522402</v>
+        <v>0</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>23494299</v>
+        <v>0</v>
       </c>
       <c r="G2" s="1" t="n">
-        <v>7028103</v>
-      </c>
-      <c r="H2" t="n">
-        <v>6168802</v>
+        <v>0</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>7028103</v>
+        <v>0</v>
       </c>
       <c r="J2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K2" s="1" t="inlineStr">
+      <c r="K2" s="3" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -554,27 +557,27 @@
           <t>AC11</t>
         </is>
       </c>
-      <c r="E3" s="2" t="n">
+      <c r="E3" s="1" t="n">
         <v>1569026</v>
       </c>
-      <c r="F3" s="2" t="n">
-        <v/>
-      </c>
-      <c r="G3" s="2" t="n">
+      <c r="F3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1" t="n">
         <v>1569026</v>
       </c>
-      <c r="H3" t="n">
+      <c r="H3" s="2" t="n">
         <v>1642584</v>
       </c>
-      <c r="I3" s="2" t="n">
-        <v/>
-      </c>
-      <c r="J3" s="2" t="n">
-        <v/>
-      </c>
-      <c r="K3" s="2" t="inlineStr">
-        <is>
-          <t>NOT_OK</t>
+      <c r="I3" s="1" t="n">
+        <v>1569026</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="3" t="inlineStr">
+        <is>
+          <t>OK</t>
         </is>
       </c>
     </row>
@@ -606,7 +609,7 @@
       <c r="G4" s="1" t="n">
         <v>5444077</v>
       </c>
-      <c r="H4" t="n">
+      <c r="H4" s="2" t="n">
         <v>4511218</v>
       </c>
       <c r="I4" s="1" t="n">
@@ -615,7 +618,7 @@
       <c r="J4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K4" s="1" t="inlineStr">
+      <c r="K4" s="3" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -640,27 +643,27 @@
           <t>AC13</t>
         </is>
       </c>
-      <c r="E5" s="2" t="n">
+      <c r="E5" s="1" t="n">
         <v>15000</v>
       </c>
-      <c r="F5" s="2" t="n">
-        <v/>
-      </c>
-      <c r="G5" s="2" t="n">
+      <c r="F5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1" t="n">
         <v>15000</v>
       </c>
-      <c r="H5" t="n">
+      <c r="H5" s="2" t="n">
         <v>15000</v>
       </c>
-      <c r="I5" s="2" t="n">
-        <v/>
-      </c>
-      <c r="J5" s="2" t="n">
-        <v/>
-      </c>
-      <c r="K5" s="2" t="inlineStr">
-        <is>
-          <t>NOT_OK</t>
+      <c r="I5" s="1" t="n">
+        <v>15000</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="3" t="inlineStr">
+        <is>
+          <t>OK</t>
         </is>
       </c>
     </row>
@@ -684,24 +687,24 @@
         </is>
       </c>
       <c r="E6" s="1" t="n">
-        <v>25469451</v>
+        <v>0</v>
       </c>
       <c r="F6" s="1" t="n">
-        <v>22954838</v>
+        <v>0</v>
       </c>
       <c r="G6" s="1" t="n">
-        <v>2514613</v>
-      </c>
-      <c r="H6" t="n">
-        <v>3007055</v>
+        <v>0</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="I6" s="1" t="n">
-        <v>2514613</v>
+        <v>0</v>
       </c>
       <c r="J6" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K6" s="1" t="inlineStr">
+      <c r="K6" s="3" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -735,7 +738,7 @@
       <c r="G7" s="1" t="n">
         <v>2455766</v>
       </c>
-      <c r="H7" t="n">
+      <c r="H7" s="2" t="n">
         <v>2919081</v>
       </c>
       <c r="I7" s="1" t="n">
@@ -744,7 +747,7 @@
       <c r="J7" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K7" s="1" t="inlineStr">
+      <c r="K7" s="3" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -778,7 +781,7 @@
       <c r="G8" s="1" t="n">
         <v>58847</v>
       </c>
-      <c r="H8" t="n">
+      <c r="H8" s="2" t="n">
         <v>87974</v>
       </c>
       <c r="I8" s="1" t="n">
@@ -787,7 +790,7 @@
       <c r="J8" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="K8" s="1" t="inlineStr">
+      <c r="K8" s="3" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -813,24 +816,24 @@
         </is>
       </c>
       <c r="E9" s="1" t="n">
-        <v>925260311</v>
+        <v>0</v>
       </c>
       <c r="F9" s="1" t="n">
-        <v>97499808</v>
+        <v>0</v>
       </c>
       <c r="G9" s="1" t="n">
-        <v>827760503</v>
-      </c>
-      <c r="H9" t="n">
-        <v>767408450</v>
+        <v>0</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="I9" s="1" t="n">
-        <v>827760503</v>
+        <v>0</v>
       </c>
       <c r="J9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K9" s="1" t="inlineStr">
+      <c r="K9" s="3" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -864,7 +867,7 @@
       <c r="G10" s="1" t="n">
         <v>57398634</v>
       </c>
-      <c r="H10" t="n">
+      <c r="H10" s="2" t="n">
         <v>53558944</v>
       </c>
       <c r="I10" s="1" t="n">
@@ -873,7 +876,7 @@
       <c r="J10" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K10" s="1" t="inlineStr">
+      <c r="K10" s="3" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -907,7 +910,7 @@
       <c r="G11" s="1" t="n">
         <v>5500463</v>
       </c>
-      <c r="H11" t="n">
+      <c r="H11" s="2" t="n">
         <v>7207850</v>
       </c>
       <c r="I11" s="1" t="n">
@@ -916,7 +919,7 @@
       <c r="J11" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K11" s="1" t="inlineStr">
+      <c r="K11" s="3" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -950,7 +953,7 @@
       <c r="G12" s="1" t="n">
         <v>51898171</v>
       </c>
-      <c r="H12" t="n">
+      <c r="H12" s="2" t="n">
         <v>46351094</v>
       </c>
       <c r="I12" s="1" t="n">
@@ -959,7 +962,7 @@
       <c r="J12" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K12" s="1" t="inlineStr">
+      <c r="K12" s="3" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -993,7 +996,7 @@
       <c r="G13" s="1" t="n">
         <v>309265295</v>
       </c>
-      <c r="H13" t="n">
+      <c r="H13" s="2" t="n">
         <v>308215255</v>
       </c>
       <c r="I13" s="1" t="n">
@@ -1002,7 +1005,7 @@
       <c r="J13" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K13" s="1" t="inlineStr">
+      <c r="K13" s="3" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -1036,7 +1039,7 @@
       <c r="G14" s="1" t="n">
         <v>64145836</v>
       </c>
-      <c r="H14" t="n">
+      <c r="H14" s="2" t="n">
         <v>65048030</v>
       </c>
       <c r="I14" s="1" t="n">
@@ -1045,7 +1048,7 @@
       <c r="J14" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K14" s="1" t="inlineStr">
+      <c r="K14" s="3" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -1079,7 +1082,7 @@
       <c r="G15" s="1" t="n">
         <v>211353259</v>
       </c>
-      <c r="H15" t="n">
+      <c r="H15" s="2" t="n">
         <v>207278054</v>
       </c>
       <c r="I15" s="1" t="n">
@@ -1088,7 +1091,7 @@
       <c r="J15" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K15" s="1" t="inlineStr">
+      <c r="K15" s="3" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -1113,27 +1116,27 @@
           <t>AC324</t>
         </is>
       </c>
-      <c r="E16" s="2" t="n">
+      <c r="E16" s="1" t="n">
         <v>33766200</v>
       </c>
-      <c r="F16" s="2" t="n">
-        <v/>
-      </c>
-      <c r="G16" s="2" t="n">
+      <c r="F16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1" t="n">
         <v>33766200</v>
       </c>
-      <c r="H16" t="n">
+      <c r="H16" s="2" t="n">
         <v>35889170</v>
       </c>
-      <c r="I16" s="2" t="n">
-        <v/>
-      </c>
-      <c r="J16" s="2" t="n">
-        <v/>
-      </c>
-      <c r="K16" s="2" t="inlineStr">
-        <is>
-          <t>NOT_OK</t>
+      <c r="I16" s="1" t="n">
+        <v>33766200</v>
+      </c>
+      <c r="J16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" s="3" t="inlineStr">
+        <is>
+          <t>OK</t>
         </is>
       </c>
     </row>
@@ -1165,7 +1168,7 @@
       <c r="G17" s="1" t="n">
         <v>445994361</v>
       </c>
-      <c r="H17" t="n">
+      <c r="H17" s="2" t="n">
         <v>391157949</v>
       </c>
       <c r="I17" s="1" t="n">
@@ -1174,7 +1177,7 @@
       <c r="J17" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K17" s="1" t="inlineStr">
+      <c r="K17" s="3" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -1208,7 +1211,7 @@
       <c r="G18" s="1" t="n">
         <v>43555363</v>
       </c>
-      <c r="H18" t="n">
+      <c r="H18" s="2" t="n">
         <v>39226410</v>
       </c>
       <c r="I18" s="1" t="n">
@@ -1217,7 +1220,7 @@
       <c r="J18" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K18" s="1" t="inlineStr">
+      <c r="K18" s="3" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -1251,7 +1254,7 @@
       <c r="G19" s="1" t="n">
         <v>240858952</v>
       </c>
-      <c r="H19" t="n">
+      <c r="H19" s="2" t="n">
         <v>222528350</v>
       </c>
       <c r="I19" s="1" t="n">
@@ -1260,7 +1263,7 @@
       <c r="J19" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K19" s="1" t="inlineStr">
+      <c r="K19" s="3" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -1294,7 +1297,7 @@
       <c r="G20" s="1" t="n">
         <v>8076894</v>
       </c>
-      <c r="H20" t="n">
+      <c r="H20" s="2" t="n">
         <v>7400037</v>
       </c>
       <c r="I20" s="1" t="n">
@@ -1303,7 +1306,7 @@
       <c r="J20" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K20" s="1" t="inlineStr">
+      <c r="K20" s="3" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -1328,25 +1331,25 @@
           <t>AC335</t>
         </is>
       </c>
-      <c r="E21" s="2" t="n">
+      <c r="E21" s="4" t="n">
         <v>153500000</v>
       </c>
-      <c r="F21" s="2" t="n">
+      <c r="F21" s="4" t="n">
         <v>153500000</v>
       </c>
-      <c r="G21" s="2" t="n">
+      <c r="G21" s="4" t="n">
         <v>122000000</v>
       </c>
-      <c r="H21" t="n">
-        <v/>
-      </c>
-      <c r="I21" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J21" s="2" t="n">
+      <c r="H21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" s="4" t="n">
         <v>122000000</v>
       </c>
-      <c r="K21" s="2" t="inlineStr">
+      <c r="K21" s="5" t="inlineStr">
         <is>
           <t>NOT_OK</t>
         </is>
@@ -1371,25 +1374,25 @@
           <t>AC336</t>
         </is>
       </c>
-      <c r="E22" s="2" t="n">
+      <c r="E22" s="4" t="n">
         <v>3152</v>
       </c>
-      <c r="F22" s="2" t="n">
+      <c r="F22" s="4" t="n">
         <v>3152</v>
       </c>
-      <c r="G22" s="2" t="n">
+      <c r="G22" s="4" t="n">
         <v>3152</v>
       </c>
-      <c r="H22" t="n">
-        <v/>
-      </c>
-      <c r="I22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J22" s="2" t="n">
+      <c r="H22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" s="4" t="n">
         <v>3152</v>
       </c>
-      <c r="K22" s="2" t="inlineStr">
+      <c r="K22" s="5" t="inlineStr">
         <is>
           <t>NOT_OK</t>
         </is>
@@ -1414,25 +1417,25 @@
           <t>AC34</t>
         </is>
       </c>
-      <c r="E23" s="2" t="n">
+      <c r="E23" s="4" t="n">
         <v>15102214</v>
       </c>
-      <c r="F23" s="2" t="n">
+      <c r="F23" s="4" t="n">
         <v>15102214</v>
       </c>
-      <c r="G23" s="2" t="n">
+      <c r="G23" s="4" t="n">
         <v>14476302</v>
       </c>
-      <c r="H23" t="n">
-        <v/>
-      </c>
-      <c r="I23" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J23" s="2" t="n">
+      <c r="H23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" s="4" t="n">
         <v>14476302</v>
       </c>
-      <c r="K23" s="2" t="inlineStr">
+      <c r="K23" s="5" t="inlineStr">
         <is>
           <t>NOT_OK</t>
         </is>
@@ -1457,27 +1460,27 @@
           <t>AC5</t>
         </is>
       </c>
-      <c r="E24" s="2" t="n">
-        <v>90077227</v>
-      </c>
-      <c r="F24" s="2" t="n">
-        <v/>
-      </c>
-      <c r="G24" s="2" t="n">
-        <v>90077227</v>
-      </c>
-      <c r="H24" t="n">
-        <v>85350986</v>
-      </c>
-      <c r="I24" s="2" t="n">
-        <v/>
-      </c>
-      <c r="J24" s="2" t="n">
-        <v/>
-      </c>
-      <c r="K24" s="2" t="inlineStr">
-        <is>
-          <t>NOT_OK</t>
+      <c r="E24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K24" s="3" t="inlineStr">
+        <is>
+          <t>OK</t>
         </is>
       </c>
     </row>
@@ -1500,25 +1503,25 @@
           <t>AC510</t>
         </is>
       </c>
-      <c r="E25" s="2" t="n">
+      <c r="E25" s="4" t="n">
         <v>11487742</v>
       </c>
-      <c r="F25" s="2" t="n">
+      <c r="F25" s="4" t="n">
         <v>11487742</v>
       </c>
-      <c r="G25" s="2" t="n">
+      <c r="G25" s="4" t="n">
         <v>11392669</v>
       </c>
-      <c r="H25" t="n">
-        <v/>
-      </c>
-      <c r="I25" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J25" s="2" t="n">
+      <c r="H25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" s="4" t="n">
         <v>11392669</v>
       </c>
-      <c r="K25" s="2" t="inlineStr">
+      <c r="K25" s="5" t="inlineStr">
         <is>
           <t>NOT_OK</t>
         </is>
@@ -1543,25 +1546,25 @@
           <t>AC530</t>
         </is>
       </c>
-      <c r="E26" s="2" t="n">
-        <v/>
-      </c>
-      <c r="F26" s="2" t="n">
+      <c r="E26" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="4" t="n">
         <v>810930</v>
       </c>
-      <c r="G26" s="2" t="n">
-        <v/>
-      </c>
-      <c r="H26" t="n">
-        <v/>
-      </c>
-      <c r="I26" s="2" t="n">
-        <v/>
-      </c>
-      <c r="J26" s="2" t="n">
-        <v/>
-      </c>
-      <c r="K26" s="2" t="inlineStr">
+      <c r="G26" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" s="4" t="n">
+        <v>-810930</v>
+      </c>
+      <c r="J26" s="4" t="n">
+        <v>810930</v>
+      </c>
+      <c r="K26" s="5" t="inlineStr">
         <is>
           <t>NOT_OK</t>
         </is>
@@ -1586,25 +1589,25 @@
           <t>AC531</t>
         </is>
       </c>
-      <c r="E27" s="2" t="n">
+      <c r="E27" s="4" t="n">
         <v>78589485</v>
       </c>
-      <c r="F27" s="2" t="n">
+      <c r="F27" s="4" t="n">
         <v>78589485</v>
       </c>
-      <c r="G27" s="2" t="n">
+      <c r="G27" s="4" t="n">
         <v>73147387</v>
       </c>
-      <c r="H27" t="n">
-        <v/>
-      </c>
-      <c r="I27" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J27" s="2" t="n">
+      <c r="H27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" s="4" t="n">
         <v>73147387</v>
       </c>
-      <c r="K27" s="2" t="inlineStr">
+      <c r="K27" s="5" t="inlineStr">
         <is>
           <t>NOT_OK</t>
         </is>
@@ -1630,24 +1633,24 @@
         </is>
       </c>
       <c r="E28" s="1" t="n">
-        <v>236075998</v>
+        <v>0</v>
       </c>
       <c r="F28" s="1" t="n">
-        <v>63569170</v>
+        <v>0</v>
       </c>
       <c r="G28" s="1" t="n">
-        <v>172506829</v>
-      </c>
-      <c r="H28" t="n">
-        <v>141530534</v>
+        <v>0</v>
+      </c>
+      <c r="H28" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="I28" s="1" t="n">
-        <v>172506828</v>
+        <v>0</v>
       </c>
       <c r="J28" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="K28" s="1" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="K28" s="3" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -1681,7 +1684,7 @@
       <c r="G29" s="1" t="n">
         <v>94917391</v>
       </c>
-      <c r="H29" t="n">
+      <c r="H29" s="2" t="n">
         <v>80250399</v>
       </c>
       <c r="I29" s="1" t="n">
@@ -1690,7 +1693,7 @@
       <c r="J29" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K29" s="1" t="inlineStr">
+      <c r="K29" s="3" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -1715,25 +1718,25 @@
           <t>AC611</t>
         </is>
       </c>
-      <c r="E30" s="2" t="n">
+      <c r="E30" s="4" t="n">
         <v>11653842</v>
       </c>
-      <c r="F30" s="2" t="n">
+      <c r="F30" s="4" t="n">
         <v>11653842</v>
       </c>
-      <c r="G30" s="2" t="n">
+      <c r="G30" s="4" t="n">
         <v>11915413</v>
       </c>
-      <c r="H30" t="n">
-        <v/>
-      </c>
-      <c r="I30" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J30" s="2" t="n">
+      <c r="H30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" s="4" t="n">
         <v>11915413</v>
       </c>
-      <c r="K30" s="2" t="inlineStr">
+      <c r="K30" s="5" t="inlineStr">
         <is>
           <t>NOT_OK</t>
         </is>
@@ -1767,7 +1770,7 @@
       <c r="G31" s="1" t="n">
         <v>56162920</v>
       </c>
-      <c r="H31" t="n">
+      <c r="H31" s="2" t="n">
         <v>48509362</v>
       </c>
       <c r="I31" s="1" t="n">
@@ -1776,7 +1779,7 @@
       <c r="J31" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K31" s="1" t="inlineStr">
+      <c r="K31" s="3" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -1810,7 +1813,7 @@
       <c r="G32" s="1" t="n">
         <v>27100629</v>
       </c>
-      <c r="H32" t="n">
+      <c r="H32" s="2" t="n">
         <v>19825624</v>
       </c>
       <c r="I32" s="1" t="n">
@@ -1819,7 +1822,7 @@
       <c r="J32" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K32" s="1" t="inlineStr">
+      <c r="K32" s="3" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -1853,7 +1856,7 @@
       <c r="G33" s="1" t="n">
         <v>64124653</v>
       </c>
-      <c r="H33" t="n">
+      <c r="H33" s="2" t="n">
         <v>58229967</v>
       </c>
       <c r="I33" s="1" t="n">
@@ -1862,7 +1865,7 @@
       <c r="J33" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="K33" s="1" t="inlineStr">
+      <c r="K33" s="3" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -1896,7 +1899,7 @@
       <c r="G34" s="1" t="n">
         <v>13464785</v>
       </c>
-      <c r="H34" t="n">
+      <c r="H34" s="2" t="n">
         <v>3050168</v>
       </c>
       <c r="I34" s="1" t="n">
@@ -1905,7 +1908,7 @@
       <c r="J34" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K34" s="1" t="inlineStr">
+      <c r="K34" s="3" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -1939,7 +1942,7 @@
       <c r="G35" s="1" t="n">
         <v>10993</v>
       </c>
-      <c r="H35" t="n">
+      <c r="H35" s="2" t="n">
         <v>119735</v>
       </c>
       <c r="I35" s="1" t="n">
@@ -1948,7 +1951,7 @@
       <c r="J35" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="K35" s="1" t="inlineStr">
+      <c r="K35" s="3" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -1973,25 +1976,25 @@
           <t>AC632</t>
         </is>
       </c>
-      <c r="E36" s="2" t="n">
+      <c r="E36" s="4" t="n">
         <v>11223990</v>
       </c>
-      <c r="F36" s="2" t="n">
+      <c r="F36" s="4" t="n">
         <v>11223990</v>
       </c>
-      <c r="G36" s="2" t="n">
+      <c r="G36" s="4" t="n">
         <v>36160</v>
       </c>
-      <c r="H36" t="n">
-        <v/>
-      </c>
-      <c r="I36" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J36" s="2" t="n">
+      <c r="H36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I36" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J36" s="4" t="n">
         <v>36160</v>
       </c>
-      <c r="K36" s="2" t="inlineStr">
+      <c r="K36" s="5" t="inlineStr">
         <is>
           <t>NOT_OK</t>
         </is>
@@ -2025,7 +2028,7 @@
       <c r="G37" s="1" t="n">
         <v>2229803</v>
       </c>
-      <c r="H37" t="n">
+      <c r="H37" s="2" t="n">
         <v>2894272</v>
       </c>
       <c r="I37" s="1" t="n">
@@ -2034,7 +2037,7 @@
       <c r="J37" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K37" s="1" t="inlineStr">
+      <c r="K37" s="3" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -2059,27 +2062,27 @@
           <t>AC7</t>
         </is>
       </c>
-      <c r="E38" s="2" t="n">
-        <v>45504869</v>
-      </c>
-      <c r="F38" s="2" t="n">
-        <v/>
-      </c>
-      <c r="G38" s="2" t="n">
-        <v>45504869</v>
-      </c>
-      <c r="H38" t="n">
-        <v>40161211</v>
-      </c>
-      <c r="I38" s="2" t="n">
-        <v/>
-      </c>
-      <c r="J38" s="2" t="n">
-        <v/>
-      </c>
-      <c r="K38" s="2" t="inlineStr">
-        <is>
-          <t>NOT_OK</t>
+      <c r="E38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K38" s="3" t="inlineStr">
+        <is>
+          <t>OK</t>
         </is>
       </c>
     </row>
@@ -2102,25 +2105,25 @@
           <t>AC71</t>
         </is>
       </c>
-      <c r="E39" s="2" t="n">
+      <c r="E39" s="4" t="n">
         <v>10454182</v>
       </c>
-      <c r="F39" s="2" t="n">
+      <c r="F39" s="4" t="n">
         <v>10454182</v>
       </c>
-      <c r="G39" s="2" t="n">
+      <c r="G39" s="4" t="n">
         <v>7074988</v>
       </c>
-      <c r="H39" t="n">
-        <v/>
-      </c>
-      <c r="I39" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J39" s="2" t="n">
+      <c r="H39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I39" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" s="4" t="n">
         <v>7074988</v>
       </c>
-      <c r="K39" s="2" t="inlineStr">
+      <c r="K39" s="5" t="inlineStr">
         <is>
           <t>NOT_OK</t>
         </is>
@@ -2145,25 +2148,25 @@
           <t>AC72</t>
         </is>
       </c>
-      <c r="E40" s="2" t="n">
+      <c r="E40" s="4" t="n">
         <v>12494585</v>
       </c>
-      <c r="F40" s="2" t="n">
+      <c r="F40" s="4" t="n">
         <v>12494585</v>
       </c>
-      <c r="G40" s="2" t="n">
+      <c r="G40" s="4" t="n">
         <v>12661333</v>
       </c>
-      <c r="H40" t="n">
-        <v/>
-      </c>
-      <c r="I40" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J40" s="2" t="n">
+      <c r="H40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I40" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J40" s="4" t="n">
         <v>12661333</v>
       </c>
-      <c r="K40" s="2" t="inlineStr">
+      <c r="K40" s="5" t="inlineStr">
         <is>
           <t>NOT_OK</t>
         </is>
@@ -2188,27 +2191,27 @@
           <t>AC73</t>
         </is>
       </c>
-      <c r="E41" s="2" t="n">
+      <c r="E41" s="1" t="n">
         <v>22471672</v>
       </c>
-      <c r="F41" s="2" t="n">
-        <v/>
-      </c>
-      <c r="G41" s="2" t="n">
+      <c r="F41" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" s="1" t="n">
         <v>22471672</v>
       </c>
-      <c r="H41" t="n">
+      <c r="H41" s="2" t="n">
         <v>20402260</v>
       </c>
-      <c r="I41" s="2" t="n">
-        <v/>
-      </c>
-      <c r="J41" s="2" t="n">
-        <v/>
-      </c>
-      <c r="K41" s="2" t="inlineStr">
-        <is>
-          <t>NOT_OK</t>
+      <c r="I41" s="1" t="n">
+        <v>22471672</v>
+      </c>
+      <c r="J41" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K41" s="3" t="inlineStr">
+        <is>
+          <t>OK</t>
         </is>
       </c>
     </row>
@@ -2231,27 +2234,27 @@
           <t>AC731</t>
         </is>
       </c>
-      <c r="E42" s="2" t="n">
+      <c r="E42" s="1" t="n">
         <v>13102000</v>
       </c>
-      <c r="F42" s="2" t="n">
-        <v/>
-      </c>
-      <c r="G42" s="2" t="n">
+      <c r="F42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" s="1" t="n">
         <v>13102000</v>
       </c>
-      <c r="H42" t="n">
+      <c r="H42" s="2" t="n">
         <v>12439585</v>
       </c>
-      <c r="I42" s="2" t="n">
-        <v/>
-      </c>
-      <c r="J42" s="2" t="n">
-        <v/>
-      </c>
-      <c r="K42" s="2" t="inlineStr">
-        <is>
-          <t>NOT_OK</t>
+      <c r="I42" s="1" t="n">
+        <v>13102000</v>
+      </c>
+      <c r="J42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K42" s="3" t="inlineStr">
+        <is>
+          <t>OK</t>
         </is>
       </c>
     </row>
@@ -2274,25 +2277,25 @@
           <t>AC733</t>
         </is>
       </c>
-      <c r="E43" s="2" t="n">
+      <c r="E43" s="4" t="n">
         <v>9369672</v>
       </c>
-      <c r="F43" s="2" t="n">
+      <c r="F43" s="4" t="n">
         <v>9369672</v>
       </c>
-      <c r="G43" s="2" t="n">
+      <c r="G43" s="4" t="n">
         <v>7962675</v>
       </c>
-      <c r="H43" t="n">
-        <v/>
-      </c>
-      <c r="I43" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J43" s="2" t="n">
+      <c r="H43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I43" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J43" s="4" t="n">
         <v>7962675</v>
       </c>
-      <c r="K43" s="2" t="inlineStr">
+      <c r="K43" s="5" t="inlineStr">
         <is>
           <t>NOT_OK</t>
         </is>
@@ -2317,25 +2320,25 @@
           <t>AC75</t>
         </is>
       </c>
-      <c r="E44" s="2" t="n">
+      <c r="E44" s="4" t="n">
         <v>84430</v>
       </c>
-      <c r="F44" s="2" t="n">
+      <c r="F44" s="4" t="n">
         <v>84430</v>
       </c>
-      <c r="G44" s="2" t="n">
+      <c r="G44" s="4" t="n">
         <v>22630</v>
       </c>
-      <c r="H44" t="n">
-        <v/>
-      </c>
-      <c r="I44" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J44" s="2" t="n">
+      <c r="H44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I44" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J44" s="4" t="n">
         <v>22630</v>
       </c>
-      <c r="K44" s="2" t="inlineStr">
+      <c r="K44" s="5" t="inlineStr">
         <is>
           <t>NOT_OK</t>
         </is>
@@ -2355,6 +2358,9 @@
           <t>TOTAL  DE  L'ACTIF</t>
         </is>
       </c>
+      <c r="D45" t="n">
+        <v/>
+      </c>
       <c r="E45" s="1" t="n">
         <v>1352910258</v>
       </c>
@@ -2364,7 +2370,7 @@
       <c r="G45" s="1" t="n">
         <v>1145392144</v>
       </c>
-      <c r="H45" t="n">
+      <c r="H45" s="2" t="n">
         <v>1043627038</v>
       </c>
       <c r="I45" s="1" t="n">
@@ -2373,7 +2379,7 @@
       <c r="J45" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K45" s="1" t="inlineStr">
+      <c r="K45" s="3" t="inlineStr">
         <is>
           <t>OK</t>
         </is>

</xml_diff>